<commit_message>
more on qb and tv
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="18">
   <si>
     <t xml:space="preserve">ConnectionID</t>
   </si>
@@ -26,31 +26,34 @@
     <t xml:space="preserve">Port</t>
   </si>
   <si>
+    <t xml:space="preserve">DatabaseName</t>
+  </si>
+  <si>
     <t xml:space="preserve">Username</t>
   </si>
   <si>
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">localhost</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.86.92.30</t>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.0.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1488</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testUser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testPass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
 </sst>
 </file>
@@ -64,20 +67,20 @@
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <family val="9"/>
       <color rgb="FF000000"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
+      <family val="24"/>
+      <color rgb="FFFFFFFF"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="DengXian"/>
+      <family val="30"/>
       <color rgb="FF000000"/>
     </font>
   </fonts>
@@ -95,7 +98,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF4490C4"/>
+        <fgColor rgb="FF595959"/>
       </patternFill>
     </fill>
     <fill>
@@ -157,39 +160,48 @@
       <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
+      <c r="F1" t="s" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" outlineLevel="0" hidden="false" customHeight="false" ht="12.8" customFormat="false">
       <c r="A2" t="s" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s" s="1">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s" s="1">
+        <v>11</v>
       </c>
     </row>
     <row r="3" outlineLevel="0" hidden="false" customHeight="false" ht="12.8" customFormat="false">
       <c r="A3" t="s" s="2">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="2">
         <v>10</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="F3" t="s" s="2">
         <v>11</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more on qb and qe
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,52 +8,22 @@
     <workbookView activeTab="0" firstSheet="0" tabRatio="500" windowHeight="8192" windowWidth="16384" yWindow="0" xWindow="0" showSheetTabs="true" showVerticalScroll="true" showHorizontalScroll="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId3" sheetId="1" name="query1"/>
+    <sheet r:id="rId3" sheetId="1" name="queyr1"/>
   </sheets>
   <calcPr iterateDelta="0.001" iterate="false" refMode="A1" iterateCount="100"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3" count="4">
+  <si>
+    <t xml:space="preserve">ReportID</t>
+  </si>
   <si>
     <t xml:space="preserve">ConnectionID</t>
   </si>
   <si>
     <t xml:space="preserve">Hostname</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Port</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DatabaseName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.0.0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1488</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testUser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">testPass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
   </si>
 </sst>
 </file>
@@ -131,7 +101,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/query1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/queyr1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
@@ -152,56 +122,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" outlineLevel="0" hidden="false" customHeight="false" ht="12.8" customFormat="false">
-      <c r="A2" t="s" s="1">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="1">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="1">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="1">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="1">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" outlineLevel="0" hidden="false" customHeight="false" ht="12.8" customFormat="false">
-      <c r="A3" t="s" s="2">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>